<commit_message>
drop down list was too short
</commit_message>
<xml_diff>
--- a/indicators/rename-folder-after-your-indicator/fill_in_metadata_here_and_rename_the_file.xlsx
+++ b/indicators/rename-folder-after-your-indicator/fill_in_metadata_here_and_rename_the_file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anders.kolstad\Github\ECindicators\indicators\rename-folder-after-your-indicator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12BE52FD-2906-4094-9BD4-76FA1BA0D757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{825D44ED-1232-4793-B497-51F87E14D845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{5774BAF6-AFFD-43CB-8AE5-DFBA2C21B702}"/>
   </bookViews>
@@ -1038,7 +1038,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1222,7 +1222,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BF4D43D9-A982-4ECC-8F32-9627C08D5144}">
           <x14:formula1>
-            <xm:f>lookup!$B$2:$B$7</xm:f>
+            <xm:f>lookup!$B$2:$B$10</xm:f>
           </x14:formula1>
           <xm:sqref>B7</xm:sqref>
         </x14:dataValidation>

</xml_diff>